<commit_message>
LR model Results Compilation
</commit_message>
<xml_diff>
--- a/results/Model_Results_Summary.xlsx
+++ b/results/Model_Results_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIML\Capstone Project Loan Processing\CodeBase\loan-processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209C3BE3-DB58-4FFB-AEF3-4403F5C47061}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB79AC8-3941-4A3F-81D3-32ECCD384272}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00CAFC6D-E7ED-4D37-8A6B-16C8E85EC937}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Model</t>
   </si>
@@ -97,6 +97,78 @@
   </si>
   <si>
     <t>NN_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_LR_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_LR_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_LR_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_LR_DummyEncoded</t>
+  </si>
+  <si>
+    <t>Std_LR_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_LR_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_LR_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_LR_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_LR_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_LR_LabelEncoded</t>
+  </si>
+  <si>
+    <t>Std_LR_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_LR_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_LR_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>RS_LR_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_LR_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_LR_DummyEncoded</t>
+  </si>
+  <si>
+    <t>RS_LR_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>RS_LR_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_LR_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>RS_LR_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_LR_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_LR_LabelEncoded</t>
+  </si>
+  <si>
+    <t>RS_LR_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>RS_LR_LabelEncoded_Binning_SMOTE</t>
   </si>
 </sst>
 </file>
@@ -112,12 +184,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,14 +210,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -448,15 +532,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D182B7-3DB9-4D4B-9816-00B95ADAB652}">
-  <dimension ref="A3:J15"/>
+  <dimension ref="A3:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.44140625" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" customWidth="1"/>
@@ -724,31 +808,31 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0.81</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>0.34</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>0.64</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>0.45</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0.19950000000000001</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0.91720000000000002</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>0.52110000000000001</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>0.8276</v>
       </c>
     </row>
@@ -878,6 +962,789 @@
       </c>
       <c r="J15">
         <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>0.88</v>
+      </c>
+      <c r="D16">
+        <v>0.59</v>
+      </c>
+      <c r="E16">
+        <v>0.23</v>
+      </c>
+      <c r="F16">
+        <v>0.34</v>
+      </c>
+      <c r="G16">
+        <v>3.3622000000000001</v>
+      </c>
+      <c r="H16">
+        <v>0.90259999999999996</v>
+      </c>
+      <c r="I16">
+        <v>3.4729999999999999</v>
+      </c>
+      <c r="J16">
+        <v>0.89939999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>0.88</v>
+      </c>
+      <c r="D17">
+        <v>0.54</v>
+      </c>
+      <c r="E17">
+        <v>0.38</v>
+      </c>
+      <c r="F17">
+        <v>0.45</v>
+      </c>
+      <c r="G17">
+        <v>2.37</v>
+      </c>
+      <c r="H17">
+        <v>0.93140000000000001</v>
+      </c>
+      <c r="I17">
+        <v>3.5110999999999999</v>
+      </c>
+      <c r="J17">
+        <v>0.89829999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>0.82</v>
+      </c>
+      <c r="D18">
+        <v>0.17</v>
+      </c>
+      <c r="E18">
+        <v>0.93</v>
+      </c>
+      <c r="F18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G18">
+        <v>11.0228</v>
+      </c>
+      <c r="H18">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="I18">
+        <v>16.983499999999999</v>
+      </c>
+      <c r="J18">
+        <v>0.50829999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>0.26</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>4.0403000000000002</v>
+      </c>
+      <c r="H19">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I19">
+        <v>3.8163999999999998</v>
+      </c>
+      <c r="J19">
+        <v>0.88949999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>0.81</v>
+      </c>
+      <c r="D20">
+        <v>0.53</v>
+      </c>
+      <c r="E20">
+        <v>0.23</v>
+      </c>
+      <c r="F20">
+        <v>0.33</v>
+      </c>
+      <c r="G20">
+        <v>3.3717000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="I20">
+        <v>3.6255999999999999</v>
+      </c>
+      <c r="J20">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>0.66</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>3.1532</v>
+      </c>
+      <c r="H21">
+        <v>0.90869999999999995</v>
+      </c>
+      <c r="I21">
+        <v>3.7401</v>
+      </c>
+      <c r="J21">
+        <v>0.89170000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>0.86</v>
+      </c>
+      <c r="D22">
+        <v>0.52</v>
+      </c>
+      <c r="E22">
+        <v>0.12</v>
+      </c>
+      <c r="F22">
+        <v>0.2</v>
+      </c>
+      <c r="G22">
+        <v>3.8492999999999999</v>
+      </c>
+      <c r="H22">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="I22">
+        <v>3.702</v>
+      </c>
+      <c r="J22">
+        <v>0.89280000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>0.86</v>
+      </c>
+      <c r="D23">
+        <v>0.33</v>
+      </c>
+      <c r="E23">
+        <v>0.73</v>
+      </c>
+      <c r="F23">
+        <v>0.46</v>
+      </c>
+      <c r="G23">
+        <v>6.1387</v>
+      </c>
+      <c r="H23">
+        <v>0.82230000000000003</v>
+      </c>
+      <c r="I23">
+        <v>6.5262000000000002</v>
+      </c>
+      <c r="J23">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>0.82</v>
+      </c>
+      <c r="D24">
+        <v>0.18</v>
+      </c>
+      <c r="E24">
+        <v>0.93</v>
+      </c>
+      <c r="F24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G24">
+        <v>10.882099999999999</v>
+      </c>
+      <c r="H24">
+        <v>0.68489999999999995</v>
+      </c>
+      <c r="I24">
+        <v>16.601900000000001</v>
+      </c>
+      <c r="J24">
+        <v>0.51929999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>0.26</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>4.0403000000000002</v>
+      </c>
+      <c r="H25">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I25">
+        <v>3.8163999999999998</v>
+      </c>
+      <c r="J25">
+        <v>0.88949999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>0.78</v>
+      </c>
+      <c r="D26">
+        <v>0.46</v>
+      </c>
+      <c r="E26">
+        <v>0.16</v>
+      </c>
+      <c r="F26">
+        <v>0.24</v>
+      </c>
+      <c r="G26">
+        <v>3.7252000000000001</v>
+      </c>
+      <c r="H26">
+        <v>0.8921</v>
+      </c>
+      <c r="I26">
+        <v>3.8546</v>
+      </c>
+      <c r="J26">
+        <v>0.88839999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>0.77</v>
+      </c>
+      <c r="D27">
+        <v>0.35</v>
+      </c>
+      <c r="E27">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F27">
+        <v>0.32</v>
+      </c>
+      <c r="G27">
+        <v>4.7107999999999999</v>
+      </c>
+      <c r="H27">
+        <v>0.86360000000000003</v>
+      </c>
+      <c r="I27">
+        <v>4.6178999999999997</v>
+      </c>
+      <c r="J27">
+        <v>0.86629999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>0.89</v>
+      </c>
+      <c r="D28">
+        <v>0.6</v>
+      </c>
+      <c r="E28">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F28">
+        <v>0.38</v>
+      </c>
+      <c r="G28">
+        <v>3.2094</v>
+      </c>
+      <c r="H28">
+        <v>0.90710000000000002</v>
+      </c>
+      <c r="I28">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="J28">
+        <v>0.90159999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>0.88</v>
+      </c>
+      <c r="D29">
+        <v>0.53</v>
+      </c>
+      <c r="E29">
+        <v>0.35</v>
+      </c>
+      <c r="F29">
+        <v>0.42</v>
+      </c>
+      <c r="G29">
+        <v>2.4447000000000001</v>
+      </c>
+      <c r="H29">
+        <v>0.92920000000000003</v>
+      </c>
+      <c r="I29">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="J29">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>0.89</v>
+      </c>
+      <c r="D30">
+        <v>0.6</v>
+      </c>
+      <c r="E30">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F30">
+        <v>0.38</v>
+      </c>
+      <c r="G30">
+        <v>1.8281000000000001</v>
+      </c>
+      <c r="H30">
+        <v>0.94710000000000005</v>
+      </c>
+      <c r="I30">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="J30">
+        <v>0.90159999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>0.89</v>
+      </c>
+      <c r="D31">
+        <v>0.6</v>
+      </c>
+      <c r="E31">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F31">
+        <v>0.38</v>
+      </c>
+      <c r="G31">
+        <v>3.2094</v>
+      </c>
+      <c r="H31">
+        <v>0.90710000000000002</v>
+      </c>
+      <c r="I31">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="J31">
+        <v>0.90169999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>0.8</v>
+      </c>
+      <c r="D32">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E32">
+        <v>0.27</v>
+      </c>
+      <c r="F32">
+        <v>0.36</v>
+      </c>
+      <c r="G32">
+        <v>3.3813</v>
+      </c>
+      <c r="H32">
+        <v>0.90210000000000001</v>
+      </c>
+      <c r="I32">
+        <v>3.5110999999999999</v>
+      </c>
+      <c r="J32">
+        <v>0.89829999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>0.79</v>
+      </c>
+      <c r="D33">
+        <v>0.51</v>
+      </c>
+      <c r="E33">
+        <v>0.3</v>
+      </c>
+      <c r="F33">
+        <v>0.37</v>
+      </c>
+      <c r="G33">
+        <v>2.0714999999999999</v>
+      </c>
+      <c r="H33">
+        <v>0.94</v>
+      </c>
+      <c r="I33">
+        <v>3.702</v>
+      </c>
+      <c r="J33">
+        <v>0.8982</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>0.87</v>
+      </c>
+      <c r="D34">
+        <v>0.52</v>
+      </c>
+      <c r="E34">
+        <v>0.17</v>
+      </c>
+      <c r="F34">
+        <v>0.26</v>
+      </c>
+      <c r="G34">
+        <v>3.7730000000000001</v>
+      </c>
+      <c r="H34">
+        <v>0.89080000000000004</v>
+      </c>
+      <c r="I34">
+        <v>3.702</v>
+      </c>
+      <c r="J34">
+        <v>0.89280000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>0.87</v>
+      </c>
+      <c r="D35">
+        <v>0.35</v>
+      </c>
+      <c r="E35">
+        <v>0.74</v>
+      </c>
+      <c r="F35">
+        <v>0.47</v>
+      </c>
+      <c r="G35">
+        <v>6.0468000000000002</v>
+      </c>
+      <c r="H35">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="I35">
+        <v>6.2210000000000001</v>
+      </c>
+      <c r="J35">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>0.84</v>
+      </c>
+      <c r="D36">
+        <v>0.34</v>
+      </c>
+      <c r="E36">
+        <v>0.65</v>
+      </c>
+      <c r="F36">
+        <v>0.44</v>
+      </c>
+      <c r="G36">
+        <v>5.1760000000000002</v>
+      </c>
+      <c r="H36">
+        <v>0.85009999999999997</v>
+      </c>
+      <c r="I36">
+        <v>6.1445999999999996</v>
+      </c>
+      <c r="J36">
+        <v>0.82210000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>0.84</v>
+      </c>
+      <c r="D37">
+        <v>0.5</v>
+      </c>
+      <c r="E37">
+        <v>0.21</v>
+      </c>
+      <c r="F37">
+        <v>0.3</v>
+      </c>
+      <c r="G37">
+        <v>3.8971</v>
+      </c>
+      <c r="H37">
+        <v>0.88719999999999999</v>
+      </c>
+      <c r="I37">
+        <v>3.7401</v>
+      </c>
+      <c r="J37">
+        <v>0.89170000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>0.78</v>
+      </c>
+      <c r="D38">
+        <v>0.46</v>
+      </c>
+      <c r="E38">
+        <v>0.16</v>
+      </c>
+      <c r="F38">
+        <v>0.24</v>
+      </c>
+      <c r="G38">
+        <v>3.7347000000000001</v>
+      </c>
+      <c r="H38">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="I38">
+        <v>3.8546</v>
+      </c>
+      <c r="J38">
+        <v>0.88839999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>0.75</v>
+      </c>
+      <c r="D39">
+        <v>0.36</v>
+      </c>
+      <c r="E39">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F39">
+        <v>0.31</v>
+      </c>
+      <c r="G39">
+        <v>4.6242999999999999</v>
+      </c>
+      <c r="H39">
+        <v>0.86609999999999998</v>
+      </c>
+      <c r="I39">
+        <v>4.5415999999999999</v>
+      </c>
+      <c r="J39">
+        <v>0.86850000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RF model Results Compilation
</commit_message>
<xml_diff>
--- a/results/Model_Results_Summary.xlsx
+++ b/results/Model_Results_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIML\Capstone Project Loan Processing\CodeBase\loan-processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB79AC8-3941-4A3F-81D3-32ECCD384272}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F5E073-E1F5-4766-9E62-92C05FDDB934}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00CAFC6D-E7ED-4D37-8A6B-16C8E85EC937}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Model</t>
   </si>
@@ -169,6 +169,78 @@
   </si>
   <si>
     <t>RS_LR_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_RF_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_RF_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_RF_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_RF_DummyEncoded</t>
+  </si>
+  <si>
+    <t>Std_RF_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_RF_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_RF_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_RF_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_RF_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_RF_LabelEncoded</t>
+  </si>
+  <si>
+    <t>Std_RF_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_RF_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_RF_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>RS_RF_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_RF_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_RF_DummyEncoded</t>
+  </si>
+  <si>
+    <t>RS_RF_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>RS_RF_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_RF_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>RS_RF_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_RF_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_RF_LabelEncoded</t>
+  </si>
+  <si>
+    <t>RS_RF_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>RS_RF_LabelEncoded_Binning_SMOTE</t>
   </si>
 </sst>
 </file>
@@ -532,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D182B7-3DB9-4D4B-9816-00B95ADAB652}">
-  <dimension ref="A3:J42"/>
+  <dimension ref="A3:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1736,15 +1808,768 @@
       <c r="A40">
         <v>37</v>
       </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>0.91</v>
+      </c>
+      <c r="D40">
+        <v>0.6</v>
+      </c>
+      <c r="E40">
+        <v>0.27</v>
+      </c>
+      <c r="F40">
+        <v>0.37</v>
+      </c>
+      <c r="G40">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="J40">
+        <v>0.91</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <v>0.9</v>
+      </c>
+      <c r="D41">
+        <v>0.43</v>
+      </c>
+      <c r="E41">
+        <v>0.42</v>
+      </c>
+      <c r="F41">
+        <v>0.42</v>
+      </c>
+      <c r="G41">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>4.2363</v>
+      </c>
+      <c r="J41">
+        <v>0.87729999999999997</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>0.91</v>
+      </c>
+      <c r="D42">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E42">
+        <v>0.32</v>
+      </c>
+      <c r="F42">
+        <v>0.41</v>
+      </c>
+      <c r="G42">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>3.4348000000000001</v>
+      </c>
+      <c r="J42">
+        <v>0.90049999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43">
+        <v>0.91</v>
+      </c>
+      <c r="D43">
+        <v>0.6</v>
+      </c>
+      <c r="E43">
+        <v>0.26</v>
+      </c>
+      <c r="F43">
+        <v>0.36</v>
+      </c>
+      <c r="G43">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>3.4348000000000001</v>
+      </c>
+      <c r="J43">
+        <v>0.90049999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>0.81</v>
+      </c>
+      <c r="D44">
+        <v>0.5</v>
+      </c>
+      <c r="E44">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F44">
+        <v>0.36</v>
+      </c>
+      <c r="G44">
+        <v>0.5444</v>
+      </c>
+      <c r="H44">
+        <v>0.98419999999999996</v>
+      </c>
+      <c r="I44">
+        <v>3.7401</v>
+      </c>
+      <c r="J44">
+        <v>0.89170000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45">
+        <v>0.82</v>
+      </c>
+      <c r="D45">
+        <v>0.44</v>
+      </c>
+      <c r="E45">
+        <v>0.36</v>
+      </c>
+      <c r="F45">
+        <v>0.4</v>
+      </c>
+      <c r="G45">
+        <v>0.31369999999999998</v>
+      </c>
+      <c r="H45">
+        <v>0.9909</v>
+      </c>
+      <c r="I45">
+        <v>4.0835999999999997</v>
+      </c>
+      <c r="J45">
+        <v>0.88180000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46">
+        <v>0.91</v>
+      </c>
+      <c r="D46">
+        <v>0.61</v>
+      </c>
+      <c r="E46">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F46">
+        <v>0.38</v>
+      </c>
+      <c r="G46">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>3.3584999999999998</v>
+      </c>
+      <c r="J46">
+        <v>0.90280000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47">
+        <v>0.9</v>
+      </c>
+      <c r="D47">
+        <v>0.4</v>
+      </c>
+      <c r="E47">
+        <v>0.51</v>
+      </c>
+      <c r="F47">
+        <v>0.45</v>
+      </c>
+      <c r="G47">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>4.6943000000000001</v>
+      </c>
+      <c r="J47">
+        <v>0.86409999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>0.89</v>
+      </c>
+      <c r="D48">
+        <v>0.45</v>
+      </c>
+      <c r="E48">
+        <v>0.54</v>
+      </c>
+      <c r="F48">
+        <v>0.49</v>
+      </c>
+      <c r="G48">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>4.2363</v>
+      </c>
+      <c r="J48">
+        <v>0.87729999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49">
+        <v>0.91</v>
+      </c>
+      <c r="D49">
+        <v>0.6</v>
+      </c>
+      <c r="E49">
+        <v>0.27</v>
+      </c>
+      <c r="F49">
+        <v>0.37</v>
+      </c>
+      <c r="G49">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="J49">
+        <v>0.90159999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50">
+        <v>0.8</v>
+      </c>
+      <c r="D50">
+        <v>0.47</v>
+      </c>
+      <c r="E50">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F50">
+        <v>0.35</v>
+      </c>
+      <c r="G50">
+        <v>0.5444</v>
+      </c>
+      <c r="H50">
+        <v>0.98419999999999996</v>
+      </c>
+      <c r="I50">
+        <v>3.8927999999999998</v>
+      </c>
+      <c r="J50">
+        <v>0.88729999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51">
+        <v>0.81</v>
+      </c>
+      <c r="D51">
+        <v>0.37</v>
+      </c>
+      <c r="E51">
+        <v>0.4</v>
+      </c>
+      <c r="F51">
+        <v>0.38</v>
+      </c>
+      <c r="G51">
+        <v>0.48139999999999999</v>
+      </c>
+      <c r="H51">
+        <v>0.98609999999999998</v>
+      </c>
+      <c r="I51">
+        <v>4.7706</v>
+      </c>
+      <c r="J51">
+        <v>0.8619</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52">
+        <v>0.92</v>
+      </c>
+      <c r="D52">
+        <v>0.53</v>
+      </c>
+      <c r="E52">
+        <v>0.17</v>
+      </c>
+      <c r="F52">
+        <v>0.26</v>
+      </c>
+      <c r="G52">
+        <v>1.3086</v>
+      </c>
+      <c r="H52">
+        <v>0.96209999999999996</v>
+      </c>
+      <c r="I52">
+        <v>3.6638000000000002</v>
+      </c>
+      <c r="J52">
+        <v>0.89390000000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53">
+        <v>0.91</v>
+      </c>
+      <c r="D53">
+        <v>0.48</v>
+      </c>
+      <c r="E53">
+        <v>0.42</v>
+      </c>
+      <c r="F53">
+        <v>0.45</v>
+      </c>
+      <c r="G53">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="H53">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="I53">
+        <v>3.8546</v>
+      </c>
+      <c r="J53">
+        <v>0.88839999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54">
+        <v>0.92</v>
+      </c>
+      <c r="D54">
+        <v>0.53</v>
+      </c>
+      <c r="E54">
+        <v>0.32</v>
+      </c>
+      <c r="F54">
+        <v>0.4</v>
+      </c>
+      <c r="G54">
+        <v>0.29210000000000003</v>
+      </c>
+      <c r="H54">
+        <v>0.99150000000000005</v>
+      </c>
+      <c r="I54">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="J54">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>0.92</v>
+      </c>
+      <c r="D55">
+        <v>0.53</v>
+      </c>
+      <c r="E55">
+        <v>0.17</v>
+      </c>
+      <c r="F55">
+        <v>0.26</v>
+      </c>
+      <c r="G55">
+        <v>1.3086</v>
+      </c>
+      <c r="H55">
+        <v>0.96209999999999996</v>
+      </c>
+      <c r="I55">
+        <v>3.6638000000000002</v>
+      </c>
+      <c r="J55">
+        <v>0.89390000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56">
+        <v>0.83</v>
+      </c>
+      <c r="D56">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E56">
+        <v>0.21</v>
+      </c>
+      <c r="F56">
+        <v>0.31</v>
+      </c>
+      <c r="G56">
+        <v>3.0087999999999999</v>
+      </c>
+      <c r="H56">
+        <v>0.91290000000000004</v>
+      </c>
+      <c r="I56">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="J56">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57">
+        <v>0.82</v>
+      </c>
+      <c r="D57">
+        <v>0.48</v>
+      </c>
+      <c r="E57">
+        <v>0.37</v>
+      </c>
+      <c r="F57">
+        <v>0.42</v>
+      </c>
+      <c r="G57">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="H57">
+        <v>0.97819999999999996</v>
+      </c>
+      <c r="I57">
+        <v>3.8546</v>
+      </c>
+      <c r="J57">
+        <v>0.88839999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <v>0.92</v>
+      </c>
+      <c r="D58">
+        <v>0.59</v>
+      </c>
+      <c r="E58">
+        <v>0.24</v>
+      </c>
+      <c r="F58">
+        <v>0.35</v>
+      </c>
+      <c r="G58">
+        <v>1.8148</v>
+      </c>
+      <c r="H58">
+        <v>0.94740000000000002</v>
+      </c>
+      <c r="I58">
+        <v>3.4729999999999999</v>
+      </c>
+      <c r="J58">
+        <v>0.89939999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59">
+        <v>0.9</v>
+      </c>
+      <c r="D59">
+        <v>0.44</v>
+      </c>
+      <c r="E59">
+        <v>0.52</v>
+      </c>
+      <c r="F59">
+        <v>0.47</v>
+      </c>
+      <c r="G59">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>4.3125999999999998</v>
+      </c>
+      <c r="J59">
+        <v>0.87509999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60">
+        <v>0.9</v>
+      </c>
+      <c r="D60">
+        <v>0.43</v>
+      </c>
+      <c r="E60">
+        <v>0.51</v>
+      </c>
+      <c r="F60">
+        <v>0.47</v>
+      </c>
+      <c r="G60">
+        <v>9.9920000000000009</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>4.3890000000000002</v>
+      </c>
+      <c r="J60">
+        <v>0.87290000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61">
+        <v>0.92</v>
+      </c>
+      <c r="D61">
+        <v>0.59</v>
+      </c>
+      <c r="E61">
+        <v>0.24</v>
+      </c>
+      <c r="F61">
+        <v>0.35</v>
+      </c>
+      <c r="G61">
+        <v>1.8148</v>
+      </c>
+      <c r="H61">
+        <v>0.94740000000000002</v>
+      </c>
+      <c r="I61">
+        <v>3.4729999999999999</v>
+      </c>
+      <c r="J61">
+        <v>0.89939999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62">
+        <v>0.81</v>
+      </c>
+      <c r="D62">
+        <v>0.53</v>
+      </c>
+      <c r="E62">
+        <v>0.23</v>
+      </c>
+      <c r="F62">
+        <v>0.33</v>
+      </c>
+      <c r="G62">
+        <v>2.407</v>
+      </c>
+      <c r="H62">
+        <v>0.93030000000000002</v>
+      </c>
+      <c r="I62">
+        <v>3.6255999999999999</v>
+      </c>
+      <c r="J62">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63">
+        <v>0.81</v>
+      </c>
+      <c r="D63">
+        <v>0.43</v>
+      </c>
+      <c r="E63">
+        <v>0.41</v>
+      </c>
+      <c r="F63">
+        <v>0.42</v>
+      </c>
+      <c r="G63">
+        <v>0.73560000000000003</v>
+      </c>
+      <c r="H63">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="I63">
+        <v>4.2363</v>
+      </c>
+      <c r="J63">
+        <v>0.87729999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SVM model Results Compilation
</commit_message>
<xml_diff>
--- a/results/Model_Results_Summary.xlsx
+++ b/results/Model_Results_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIML\Capstone Project Loan Processing\CodeBase\loan-processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F5E073-E1F5-4766-9E62-92C05FDDB934}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C6E096-9FEE-4F6E-B072-D86BACB87BE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00CAFC6D-E7ED-4D37-8A6B-16C8E85EC937}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Model</t>
   </si>
@@ -241,6 +241,42 @@
   </si>
   <si>
     <t>RS_RF_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_SVM_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_SVM_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_SVM_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_SVM_DummyEncoded</t>
+  </si>
+  <si>
+    <t>Std_SVM_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_SVM_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_SVM_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_SVM_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_SVM_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_SVM_LabelEncoded</t>
+  </si>
+  <si>
+    <t>Std_SVM_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_SVM_LabelEncoded_Binning_SMOTE</t>
   </si>
 </sst>
 </file>
@@ -604,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D182B7-3DB9-4D4B-9816-00B95ADAB652}">
-  <dimension ref="A3:J63"/>
+  <dimension ref="A3:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2572,6 +2608,390 @@
         <v>0.87729999999999997</v>
       </c>
     </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64">
+        <v>0.88</v>
+      </c>
+      <c r="D64">
+        <v>0.54</v>
+      </c>
+      <c r="E64">
+        <v>0.13</v>
+      </c>
+      <c r="F64">
+        <v>0.21</v>
+      </c>
+      <c r="G64">
+        <v>3.6774</v>
+      </c>
+      <c r="H64">
+        <v>0.89349999999999996</v>
+      </c>
+      <c r="I64">
+        <v>3.6638000000000002</v>
+      </c>
+      <c r="J64">
+        <v>0.89390000000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65">
+        <v>0.85</v>
+      </c>
+      <c r="D65">
+        <v>0.45</v>
+      </c>
+      <c r="E65">
+        <v>0.17</v>
+      </c>
+      <c r="F65">
+        <v>0.25</v>
+      </c>
+      <c r="G65">
+        <v>2.1255000000000002</v>
+      </c>
+      <c r="H65">
+        <v>0.93840000000000001</v>
+      </c>
+      <c r="I65">
+        <v>3.8927999999999998</v>
+      </c>
+      <c r="J65">
+        <v>0.88729999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66">
+        <v>0.84</v>
+      </c>
+      <c r="D66">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E66">
+        <v>0.71</v>
+      </c>
+      <c r="F66">
+        <v>0.42</v>
+      </c>
+      <c r="G66">
+        <v>8.5347000000000008</v>
+      </c>
+      <c r="H66">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="I66">
+        <v>7.4804000000000004</v>
+      </c>
+      <c r="J66">
+        <v>0.78339999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67">
+        <v>0.62</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>4.0212000000000003</v>
+      </c>
+      <c r="H67">
+        <v>0.88360000000000005</v>
+      </c>
+      <c r="I67">
+        <v>3.7783000000000002</v>
+      </c>
+      <c r="J67">
+        <v>0.89059999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68">
+        <v>0.83</v>
+      </c>
+      <c r="D68">
+        <v>0.54</v>
+      </c>
+      <c r="E68">
+        <v>0.34</v>
+      </c>
+      <c r="F68">
+        <v>0.42</v>
+      </c>
+      <c r="G68">
+        <v>3.1903000000000001</v>
+      </c>
+      <c r="H68">
+        <v>0.90759999999999996</v>
+      </c>
+      <c r="I68">
+        <v>3.5493000000000001</v>
+      </c>
+      <c r="J68">
+        <v>0.8972</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69">
+        <v>0.69</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>3.4885000000000002</v>
+      </c>
+      <c r="H69">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="I69">
+        <v>3.7401</v>
+      </c>
+      <c r="J69">
+        <v>0.89170000000000005</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70">
+        <v>0.77</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>4.0403000000000002</v>
+      </c>
+      <c r="H70">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I70">
+        <v>3.7401</v>
+      </c>
+      <c r="J70">
+        <v>0.89170000000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71">
+        <v>0.76</v>
+      </c>
+      <c r="D71">
+        <v>0.23</v>
+      </c>
+      <c r="E71">
+        <v>0.64</v>
+      </c>
+      <c r="F71">
+        <v>0.34</v>
+      </c>
+      <c r="G71">
+        <v>7.1284999999999998</v>
+      </c>
+      <c r="H71">
+        <v>0.79359999999999997</v>
+      </c>
+      <c r="I71">
+        <v>9.5412999999999997</v>
+      </c>
+      <c r="J71">
+        <v>0.72370000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72">
+        <v>0.84</v>
+      </c>
+      <c r="D72">
+        <v>0.3</v>
+      </c>
+      <c r="E72">
+        <v>0.7</v>
+      </c>
+      <c r="F72">
+        <v>0.42</v>
+      </c>
+      <c r="G72">
+        <v>8.5130999999999997</v>
+      </c>
+      <c r="H72">
+        <v>0.75349999999999995</v>
+      </c>
+      <c r="I72">
+        <v>7.3658999999999999</v>
+      </c>
+      <c r="J72">
+        <v>0.78669999999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73">
+        <v>0.69</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>4.0308000000000002</v>
+      </c>
+      <c r="H73">
+        <v>0.88329999999999997</v>
+      </c>
+      <c r="I73">
+        <v>3.7783000000000002</v>
+      </c>
+      <c r="J73">
+        <v>0.89059999999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74">
+        <v>0.7</v>
+      </c>
+      <c r="D74">
+        <v>0.67</v>
+      </c>
+      <c r="E74">
+        <v>0.04</v>
+      </c>
+      <c r="F74">
+        <v>0.08</v>
+      </c>
+      <c r="G74">
+        <v>3.9447999999999999</v>
+      </c>
+      <c r="H74">
+        <v>0.88580000000000003</v>
+      </c>
+      <c r="I74">
+        <v>3.6638000000000002</v>
+      </c>
+      <c r="J74">
+        <v>0.89390000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75">
+        <v>0.76</v>
+      </c>
+      <c r="D75">
+        <v>0.4</v>
+      </c>
+      <c r="E75">
+        <v>0.4</v>
+      </c>
+      <c r="F75">
+        <v>0.4</v>
+      </c>
+      <c r="G75">
+        <v>3.6993999999999998</v>
+      </c>
+      <c r="H75">
+        <v>0.89290000000000003</v>
+      </c>
+      <c r="I75">
+        <v>4.4653</v>
+      </c>
+      <c r="J75">
+        <v>0.87070000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
NB model Results Compilation
</commit_message>
<xml_diff>
--- a/results/Model_Results_Summary.xlsx
+++ b/results/Model_Results_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIML\Capstone Project Loan Processing\CodeBase\loan-processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C6E096-9FEE-4F6E-B072-D86BACB87BE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88BBE9B-9D2E-4AEB-826A-43F781656B17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00CAFC6D-E7ED-4D37-8A6B-16C8E85EC937}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Model</t>
   </si>
@@ -277,6 +277,42 @@
   </si>
   <si>
     <t>Std_SVM_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_NB_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_NB_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_NB_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_NB_DummyEncoded</t>
+  </si>
+  <si>
+    <t>Std_NB_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_NB_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_NB_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_NB_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_NB_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_NB_LabelEncoded</t>
+  </si>
+  <si>
+    <t>Std_NB_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_NB_LabelEncoded_Binning_SMOTE</t>
   </si>
 </sst>
 </file>
@@ -318,9 +354,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D182B7-3DB9-4D4B-9816-00B95ADAB652}">
-  <dimension ref="A3:J75"/>
+  <dimension ref="A3:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,31 +793,31 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.87</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.42</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.54</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0.48</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>0.20399999999999999</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0.92010000000000003</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>0.31830000000000003</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>0.87070000000000003</v>
       </c>
     </row>
@@ -1300,31 +1337,31 @@
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.86</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>0.33</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>0.73</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.46</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>6.1387</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <v>0.82230000000000003</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <v>6.5262000000000002</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
         <v>0.81100000000000005</v>
       </c>
     </row>
@@ -1684,31 +1721,31 @@
       <c r="A35">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>0.87</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>0.35</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>0.74</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>0.47</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>6.0468000000000002</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <v>0.82499999999999996</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="1">
         <v>6.2210000000000001</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="1">
         <v>0.82</v>
       </c>
     </row>
@@ -2676,31 +2713,31 @@
       <c r="A66">
         <v>63</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
         <v>0.84</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="1">
         <v>0.71</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="1">
         <v>0.42</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="1">
         <v>8.5347000000000008</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="1">
         <v>0.75290000000000001</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="1">
         <v>7.4804000000000004</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="1">
         <v>0.78339999999999999</v>
       </c>
     </row>
@@ -2836,31 +2873,31 @@
       <c r="A71">
         <v>68</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="1">
         <v>0.76</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>0.23</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="1">
         <v>0.64</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="1">
         <v>0.34</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="1">
         <v>7.1284999999999998</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="1">
         <v>0.79359999999999997</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="1">
         <v>9.5412999999999997</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="1">
         <v>0.72370000000000001</v>
       </c>
     </row>
@@ -2992,7 +3029,394 @@
         <v>0.87070000000000003</v>
       </c>
     </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76">
+        <v>0.75</v>
+      </c>
+      <c r="D76">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E76">
+        <v>0.39</v>
+      </c>
+      <c r="F76">
+        <v>0.32</v>
+      </c>
+      <c r="G76">
+        <v>5.6069000000000004</v>
+      </c>
+      <c r="H76">
+        <v>0.8377</v>
+      </c>
+      <c r="I76">
+        <v>6.0682</v>
+      </c>
+      <c r="J76">
+        <v>0.82430000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77">
+        <v>0.72</v>
+      </c>
+      <c r="D77">
+        <v>0.22</v>
+      </c>
+      <c r="E77">
+        <v>0.67</v>
+      </c>
+      <c r="F77">
+        <v>0.33</v>
+      </c>
+      <c r="G77">
+        <v>7.4530000000000003</v>
+      </c>
+      <c r="H77">
+        <v>0.78420000000000001</v>
+      </c>
+      <c r="I77">
+        <v>10.266400000000001</v>
+      </c>
+      <c r="J77">
+        <v>0.70279999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78">
+        <v>0.68</v>
+      </c>
+      <c r="D78">
+        <v>0.24</v>
+      </c>
+      <c r="E78">
+        <v>0.27</v>
+      </c>
+      <c r="F78">
+        <v>0.25</v>
+      </c>
+      <c r="G78">
+        <v>3.3912</v>
+      </c>
+      <c r="H78">
+        <v>0.90180000000000005</v>
+      </c>
+      <c r="I78">
+        <v>5.9154999999999998</v>
+      </c>
+      <c r="J78">
+        <v>0.82869999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79">
+        <v>0.77</v>
+      </c>
+      <c r="D79">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E79">
+        <v>0.42</v>
+      </c>
+      <c r="F79">
+        <v>0.35</v>
+      </c>
+      <c r="G79">
+        <v>5.3011999999999997</v>
+      </c>
+      <c r="H79">
+        <v>0.84650000000000003</v>
+      </c>
+      <c r="I79">
+        <v>5.9156000000000004</v>
+      </c>
+      <c r="J79">
+        <v>0.82869999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80">
+        <v>0.76</v>
+      </c>
+      <c r="D80">
+        <v>0.15</v>
+      </c>
+      <c r="E80">
+        <v>0.89</v>
+      </c>
+      <c r="F80">
+        <v>0.26</v>
+      </c>
+      <c r="G80">
+        <v>18.225000000000001</v>
+      </c>
+      <c r="H80">
+        <v>0.4723</v>
+      </c>
+      <c r="I80">
+        <v>19.0063</v>
+      </c>
+      <c r="J80">
+        <v>0.44969999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81">
+        <v>0.7</v>
+      </c>
+      <c r="D81">
+        <v>0.4</v>
+      </c>
+      <c r="E81">
+        <v>0.04</v>
+      </c>
+      <c r="F81">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G81">
+        <v>2.6987999999999999</v>
+      </c>
+      <c r="H81">
+        <v>0.92190000000000005</v>
+      </c>
+      <c r="I81">
+        <v>3.8163999999999998</v>
+      </c>
+      <c r="J81">
+        <v>0.88949999999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82">
+        <v>0.8</v>
+      </c>
+      <c r="D82">
+        <v>0.3</v>
+      </c>
+      <c r="E82">
+        <v>0.45</v>
+      </c>
+      <c r="F82">
+        <v>0.36</v>
+      </c>
+      <c r="G82">
+        <v>5.8170000000000002</v>
+      </c>
+      <c r="H82">
+        <v>0.83160000000000001</v>
+      </c>
+      <c r="I82">
+        <v>5.9919000000000002</v>
+      </c>
+      <c r="J82">
+        <v>0.82650000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83">
+        <v>0.79</v>
+      </c>
+      <c r="D83">
+        <v>0.18</v>
+      </c>
+      <c r="E83">
+        <v>0.87</v>
+      </c>
+      <c r="F83">
+        <v>0.3</v>
+      </c>
+      <c r="G83">
+        <v>9.4542999999999999</v>
+      </c>
+      <c r="H83">
+        <v>0.72629999999999995</v>
+      </c>
+      <c r="I83">
+        <v>15.3424</v>
+      </c>
+      <c r="J83">
+        <v>0.55579999999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84" t="s">
+        <v>90</v>
+      </c>
+      <c r="C84">
+        <v>0.76</v>
+      </c>
+      <c r="D84">
+        <v>0.2</v>
+      </c>
+      <c r="E84">
+        <v>0.8</v>
+      </c>
+      <c r="F84">
+        <v>0.32</v>
+      </c>
+      <c r="G84">
+        <v>8.1074999999999999</v>
+      </c>
+      <c r="H84">
+        <v>0.76529999999999998</v>
+      </c>
+      <c r="I84">
+        <v>12.5182</v>
+      </c>
+      <c r="J84">
+        <v>0.63759999999999994</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85" t="s">
+        <v>91</v>
+      </c>
+      <c r="C85">
+        <v>0.81</v>
+      </c>
+      <c r="D85">
+        <v>0.31</v>
+      </c>
+      <c r="E85">
+        <v>0.45</v>
+      </c>
+      <c r="F85">
+        <v>0.37</v>
+      </c>
+      <c r="G85">
+        <v>5.5686999999999998</v>
+      </c>
+      <c r="H85">
+        <v>0.83879999999999999</v>
+      </c>
+      <c r="I85">
+        <v>5.8010999999999999</v>
+      </c>
+      <c r="J85">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86">
+        <v>0.73</v>
+      </c>
+      <c r="D86">
+        <v>0.11</v>
+      </c>
+      <c r="E86">
+        <v>0.98</v>
+      </c>
+      <c r="F86">
+        <v>0.2</v>
+      </c>
+      <c r="G86">
+        <v>28.980399999999999</v>
+      </c>
+      <c r="H86">
+        <v>0.16089999999999999</v>
+      </c>
+      <c r="I86">
+        <v>29.578099999999999</v>
+      </c>
+      <c r="J86">
+        <v>0.14360000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87" t="s">
+        <v>93</v>
+      </c>
+      <c r="C87">
+        <v>0.71</v>
+      </c>
+      <c r="D87">
+        <v>0.11</v>
+      </c>
+      <c r="E87">
+        <v>0.91</v>
+      </c>
+      <c r="F87">
+        <v>0.2</v>
+      </c>
+      <c r="G87">
+        <v>15.847300000000001</v>
+      </c>
+      <c r="H87">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="I87">
+        <v>27.593499999999999</v>
+      </c>
+      <c r="J87">
+        <v>0.2011</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J75">
+    <sortCondition ref="A4:A75"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
H2O Auto ML Results compilation
</commit_message>
<xml_diff>
--- a/results/Model_Results_Summary.xlsx
+++ b/results/Model_Results_Summary.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIML\Capstone Project Loan Processing\CodeBase\loan-processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89989B37-DF80-486A-ACF6-F360AB8E0D39}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAD7A0C-68B6-495F-A141-6E74341DAF40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00CAFC6D-E7ED-4D37-8A6B-16C8E85EC937}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$K$111</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Model</t>
   </si>
@@ -42,9 +45,6 @@
     <t>precision</t>
   </si>
   <si>
-    <t>recall</t>
-  </si>
-  <si>
     <t>f1-score</t>
   </si>
   <si>
@@ -313,6 +313,84 @@
   </si>
   <si>
     <t>Std_NB_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>recall_1</t>
+  </si>
+  <si>
+    <t>recall_0</t>
+  </si>
+  <si>
+    <t>Std_XGB_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_XGB_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_XGB_DummyEncoded</t>
+  </si>
+  <si>
+    <t>Std_XGB_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_XGB_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_XGB_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>Std_XGB_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_XGB_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_XGB_LabelEncoded</t>
+  </si>
+  <si>
+    <t>Std_XGB_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>Std_XGB_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_XGB_DummyEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>RS_XGB_DummyEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_XGB_DummyEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_XGB_DummyEncoded</t>
+  </si>
+  <si>
+    <t>RS_XGB_DummyEncoded_Binning</t>
+  </si>
+  <si>
+    <t>RS_XGB_DummyEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_XGB_LabeEncoded_MinMaxScaling</t>
+  </si>
+  <si>
+    <t>RS_XGB_LabelEncoded_MinMaxScaling_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_XGB_LabelEncoded_SMOTE</t>
+  </si>
+  <si>
+    <t>RS_XGB_LabelEncoded</t>
+  </si>
+  <si>
+    <t>RS_XGB_LabelEncoded_Binning</t>
+  </si>
+  <si>
+    <t>RS_XGB_LabelEncoded_Binning_SMOTE</t>
+  </si>
+  <si>
+    <t>Std_XGB_DummyEncoded_MinMaxScaling_SMOTE</t>
   </si>
 </sst>
 </file>
@@ -677,25 +755,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D182B7-3DB9-4D4B-9816-00B95ADAB652}">
-  <dimension ref="A3:J87"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A3:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="51.109375" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -707,30 +786,33 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>0.86</v>
@@ -739,30 +821,33 @@
         <v>0.47</v>
       </c>
       <c r="E4">
+        <v>0.94</v>
+      </c>
+      <c r="F4">
         <v>0.43</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.45</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>4.4299999999999999E-2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.98529999999999995</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.46829999999999999</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.8851</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>0.83</v>
@@ -771,62 +856,68 @@
         <v>0.39</v>
       </c>
       <c r="E5">
+        <v>0.92</v>
+      </c>
+      <c r="F5">
         <v>0.45</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.42</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>3.7400000000000003E-2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.9859</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.57909999999999995</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.86519999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
         <v>0.87</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>0.42</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.54</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="2">
         <v>0.48</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="2">
         <v>0.20399999999999999</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="2">
         <v>0.92010000000000003</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="2">
         <v>0.31830000000000003</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="2">
         <v>0.87070000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>0.82</v>
@@ -834,31 +925,34 @@
       <c r="D7">
         <v>0.53</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F7">
         <v>0.19</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.30409999999999998</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.88880000000000003</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.32219999999999999</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.89390000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>0.75</v>
@@ -866,31 +960,34 @@
       <c r="D8">
         <v>0.43</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F8">
         <v>0.32</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.36</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.97650000000000003</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.57840000000000003</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.88070000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>0.76</v>
@@ -898,31 +995,34 @@
       <c r="D9">
         <v>0.42</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F9">
         <v>0.3</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.35</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.98670000000000002</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.55610000000000004</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.87949999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>0.84</v>
@@ -930,63 +1030,69 @@
       <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="F10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.36</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.1951</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.92120000000000002</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.29110000000000003</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.89170000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
         <v>0.81</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>0.34</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F11" s="2">
         <v>0.64</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="2">
         <v>0.45</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="2">
         <v>0.19950000000000001</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="2">
         <v>0.91720000000000002</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="2">
         <v>0.52110000000000001</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="2">
         <v>0.8276</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>0.81</v>
@@ -994,31 +1100,34 @@
       <c r="D12">
         <v>0.39</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="F12">
         <v>0.41</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.4</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.32719999999999999</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.8649</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.3533</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.86629999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>0.83</v>
@@ -1026,31 +1135,34 @@
       <c r="D13">
         <v>0.45</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="F13">
         <v>0.38</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>0.41</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.33129999999999998</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.88270000000000004</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.31219999999999998</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.88290000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>0.76</v>
@@ -1058,31 +1170,34 @@
       <c r="D14">
         <v>0.45</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F14">
         <v>0.34</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0.38</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.18</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.93530000000000002</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.36470000000000002</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.88290000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>0.74</v>
@@ -1090,31 +1205,34 @@
       <c r="D15">
         <v>0.3</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="F15">
         <v>0.49</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>0.37</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.10829999999999999</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.95989999999999998</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.5877</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>0.88</v>
@@ -1122,31 +1240,34 @@
       <c r="D16">
         <v>0.59</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F16">
         <v>0.23</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>0.34</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>3.3622000000000001</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.90259999999999996</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>3.4729999999999999</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>0.89939999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>0.88</v>
@@ -1154,31 +1275,34 @@
       <c r="D17">
         <v>0.54</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="F17">
         <v>0.38</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>0.45</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>2.37</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.93140000000000001</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>3.5110999999999999</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>0.89829999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>0.82</v>
@@ -1186,31 +1310,34 @@
       <c r="D18">
         <v>0.17</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="F18">
         <v>0.93</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>11.0228</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.68100000000000005</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>16.983499999999999</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0.50829999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>0.26</v>
@@ -1218,31 +1345,34 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19">
-        <v>0</v>
+      <c r="E19" s="2">
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>4.0403000000000002</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>0.88300000000000001</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>3.8163999999999998</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>0.88949999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>0.81</v>
@@ -1250,31 +1380,34 @@
       <c r="D20">
         <v>0.53</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F20">
         <v>0.23</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>0.33</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>3.3717000000000001</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>0.90239999999999998</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>3.6255999999999999</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>0.66</v>
@@ -1282,31 +1415,34 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21">
-        <v>0</v>
+      <c r="E21" s="2">
+        <v>1</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>3.1532</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>0.90869999999999995</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>3.7401</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>0.89170000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>0.86</v>
@@ -1314,31 +1450,34 @@
       <c r="D22">
         <v>0.52</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F22">
         <v>0.12</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>0.2</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>3.8492999999999999</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>0.88849999999999996</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>3.702</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>0.89280000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1">
         <v>0.86</v>
@@ -1347,30 +1486,33 @@
         <v>0.33</v>
       </c>
       <c r="E23" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="F23" s="1">
         <v>0.73</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>0.46</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>6.1387</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>0.82230000000000003</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>6.5262000000000002</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>0.81100000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <v>0.82</v>
@@ -1378,31 +1520,34 @@
       <c r="D24">
         <v>0.18</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="F24">
         <v>0.93</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>10.882099999999999</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>0.68489999999999995</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>16.601900000000001</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>0.51929999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>0.26</v>
@@ -1410,31 +1555,34 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25">
-        <v>0</v>
+      <c r="E25" s="2">
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>4.0403000000000002</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.88300000000000001</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>3.8163999999999998</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>0.88949999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26">
         <v>0.78</v>
@@ -1442,31 +1590,34 @@
       <c r="D26">
         <v>0.46</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F26">
         <v>0.16</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>0.24</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>3.7252000000000001</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>0.8921</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>3.8546</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>0.88839999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>0.77</v>
@@ -1474,31 +1625,34 @@
       <c r="D27">
         <v>0.35</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="F27">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>0.32</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>4.7107999999999999</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>0.86360000000000003</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>4.6178999999999997</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>0.86629999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>0.89</v>
@@ -1507,30 +1661,33 @@
         <v>0.6</v>
       </c>
       <c r="E28">
+        <v>0.98</v>
+      </c>
+      <c r="F28">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>0.38</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>3.2094</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>0.90710000000000002</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>3.3965999999999998</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>0.90159999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>0.88</v>
@@ -1539,30 +1696,33 @@
         <v>0.53</v>
       </c>
       <c r="E29">
+        <v>0.96</v>
+      </c>
+      <c r="F29">
         <v>0.35</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>0.42</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>2.4447000000000001</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>0.92920000000000003</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>3.5874999999999999</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>0.89610000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30">
         <v>0.89</v>
@@ -1571,30 +1731,33 @@
         <v>0.6</v>
       </c>
       <c r="E30">
+        <v>0.98</v>
+      </c>
+      <c r="F30">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>0.38</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>1.8281000000000001</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>0.94710000000000005</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>3.3965999999999998</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>0.90159999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>0.89</v>
@@ -1603,30 +1766,33 @@
         <v>0.6</v>
       </c>
       <c r="E31">
+        <v>0.98</v>
+      </c>
+      <c r="F31">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>0.38</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>3.2094</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>0.90710000000000002</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>3.3965999999999998</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>0.90169999999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32">
         <v>0.8</v>
@@ -1635,30 +1801,33 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="E32">
+        <v>0.98</v>
+      </c>
+      <c r="F32">
         <v>0.27</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>0.36</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>3.3813</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>0.90210000000000001</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>3.5110999999999999</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>0.89829999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33">
         <v>0.79</v>
@@ -1667,30 +1836,33 @@
         <v>0.51</v>
       </c>
       <c r="E33">
+        <v>0.97</v>
+      </c>
+      <c r="F33">
         <v>0.3</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>0.37</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>2.0714999999999999</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>0.94</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>3.702</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>0.8982</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>0.87</v>
@@ -1699,30 +1871,33 @@
         <v>0.52</v>
       </c>
       <c r="E34">
+        <v>0.98</v>
+      </c>
+      <c r="F34">
         <v>0.17</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>0.26</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>3.7730000000000001</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>0.89080000000000004</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>3.702</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>0.89280000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="1">
         <v>0.87</v>
@@ -1731,30 +1906,33 @@
         <v>0.35</v>
       </c>
       <c r="E35" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="F35" s="1">
         <v>0.74</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>0.47</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>6.0468000000000002</v>
       </c>
-      <c r="H35" s="1">
+      <c r="I35" s="1">
         <v>0.82499999999999996</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>6.2210000000000001</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <v>0.82</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>0.84</v>
@@ -1762,31 +1940,34 @@
       <c r="D36">
         <v>0.34</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="F36">
         <v>0.65</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>0.44</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>5.1760000000000002</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>0.85009999999999997</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>6.1445999999999996</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>0.82210000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>0.84</v>
@@ -1794,31 +1975,34 @@
       <c r="D37">
         <v>0.5</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="F37">
         <v>0.21</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>0.3</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>3.8971</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>0.88719999999999999</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>3.7401</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>0.89170000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>0.78</v>
@@ -1826,31 +2010,34 @@
       <c r="D38">
         <v>0.46</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F38">
         <v>0.16</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>0.24</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>3.7347000000000001</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>0.89200000000000002</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>3.8546</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>0.88839999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>0.75</v>
@@ -1858,31 +2045,34 @@
       <c r="D39">
         <v>0.36</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="F39">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>0.31</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>4.6242999999999999</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>0.86609999999999998</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>4.5415999999999999</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>0.86850000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>0.91</v>
@@ -1890,31 +2080,34 @@
       <c r="D40">
         <v>0.6</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F40">
         <v>0.27</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>0.37</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>1</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>3.3965999999999998</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>0.91</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>0.9</v>
@@ -1922,31 +2115,34 @@
       <c r="D41">
         <v>0.43</v>
       </c>
-      <c r="E41">
-        <v>0.42</v>
+      <c r="E41" s="2">
+        <v>0.93</v>
       </c>
       <c r="F41">
         <v>0.42</v>
       </c>
       <c r="G41">
+        <v>0.42</v>
+      </c>
+      <c r="H41">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>1</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>4.2363</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>0.87729999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>0.91</v>
@@ -1954,31 +2150,34 @@
       <c r="D42">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="F42">
         <v>0.32</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>0.41</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>1</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>3.4348000000000001</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>0.90049999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43">
         <v>0.91</v>
@@ -1986,31 +2185,34 @@
       <c r="D43">
         <v>0.6</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F43">
         <v>0.26</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>0.36</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>1</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>3.4348000000000001</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>0.90049999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44">
         <v>0.81</v>
@@ -2018,31 +2220,34 @@
       <c r="D44">
         <v>0.5</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="F44">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>0.36</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>0.5444</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>0.98419999999999996</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>3.7401</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>0.89170000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>0.82</v>
@@ -2050,31 +2255,34 @@
       <c r="D45">
         <v>0.44</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F45">
         <v>0.36</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>0.4</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>0.31369999999999998</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>0.9909</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>4.0835999999999997</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>0.88180000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46">
         <v>0.91</v>
@@ -2082,31 +2290,34 @@
       <c r="D46">
         <v>0.61</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F46">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>0.38</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>1</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>3.3584999999999998</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>0.90280000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47">
         <v>0.9</v>
@@ -2114,31 +2325,34 @@
       <c r="D47">
         <v>0.4</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F47">
         <v>0.51</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>0.45</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>1</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>4.6943000000000001</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>0.86409999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48">
         <v>0.89</v>
@@ -2146,31 +2360,34 @@
       <c r="D48">
         <v>0.45</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="F48">
         <v>0.54</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>0.49</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>1</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>4.2363</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>0.87729999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49">
         <v>0.91</v>
@@ -2178,31 +2395,34 @@
       <c r="D49">
         <v>0.6</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F49">
         <v>0.27</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>0.37</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>1</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>3.3965999999999998</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>0.90159999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>0.8</v>
@@ -2210,31 +2430,34 @@
       <c r="D50">
         <v>0.47</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="F50">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>0.35</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>0.5444</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>0.98419999999999996</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>3.8927999999999998</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>0.88729999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51">
         <v>0.81</v>
@@ -2242,31 +2465,34 @@
       <c r="D51">
         <v>0.37</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="F51">
         <v>0.4</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>0.38</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>0.48139999999999999</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>0.98609999999999998</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>4.7706</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>0.8619</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52">
         <v>0.92</v>
@@ -2275,30 +2501,33 @@
         <v>0.53</v>
       </c>
       <c r="E52">
+        <v>0.98</v>
+      </c>
+      <c r="F52">
         <v>0.17</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>0.26</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>1.3086</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>0.96209999999999996</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>3.6638000000000002</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>0.89390000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53">
         <v>0.91</v>
@@ -2307,30 +2536,33 @@
         <v>0.48</v>
       </c>
       <c r="E53">
+        <v>0.95</v>
+      </c>
+      <c r="F53">
         <v>0.42</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>0.45</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>0.99980000000000002</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>3.8546</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>0.88839999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54">
         <v>0.92</v>
@@ -2339,30 +2571,33 @@
         <v>0.53</v>
       </c>
       <c r="E54">
+        <v>0.97</v>
+      </c>
+      <c r="F54">
         <v>0.32</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>0.4</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>0.29210000000000003</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>0.99150000000000005</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>3.5874999999999999</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>0.89610000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55">
         <v>0.92</v>
@@ -2371,30 +2606,33 @@
         <v>0.53</v>
       </c>
       <c r="E55">
+        <v>0.98</v>
+      </c>
+      <c r="F55">
         <v>0.17</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>0.26</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>1.3086</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>0.96209999999999996</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>3.6638000000000002</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>0.89390000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56">
         <v>0.83</v>
@@ -2403,30 +2641,33 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E56">
+        <v>0.98</v>
+      </c>
+      <c r="F56">
         <v>0.21</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>0.31</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>3.0087999999999999</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>0.91290000000000004</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>3.5874999999999999</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>0.89610000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57">
         <v>0.82</v>
@@ -2435,30 +2676,33 @@
         <v>0.48</v>
       </c>
       <c r="E57">
+        <v>0.95</v>
+      </c>
+      <c r="F57">
         <v>0.37</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>0.42</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>0.75180000000000002</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>0.97819999999999996</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>3.8546</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>0.88839999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58">
         <v>0.92</v>
@@ -2467,30 +2711,33 @@
         <v>0.59</v>
       </c>
       <c r="E58">
+        <v>0.98</v>
+      </c>
+      <c r="F58">
         <v>0.24</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>0.35</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>1.8148</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>0.94740000000000002</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>3.4729999999999999</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>0.89939999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59">
         <v>0.9</v>
@@ -2499,30 +2746,33 @@
         <v>0.44</v>
       </c>
       <c r="E59">
+        <v>0.92</v>
+      </c>
+      <c r="F59">
         <v>0.52</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>0.47</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>1</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>4.3125999999999998</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>0.87509999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60">
         <v>0.9</v>
@@ -2531,30 +2781,33 @@
         <v>0.43</v>
       </c>
       <c r="E60">
+        <v>0.92</v>
+      </c>
+      <c r="F60">
         <v>0.51</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>0.47</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>9.9920000000000009</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>1</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>4.3890000000000002</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>0.87290000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61">
         <v>0.92</v>
@@ -2563,30 +2816,33 @@
         <v>0.59</v>
       </c>
       <c r="E61">
+        <v>0.98</v>
+      </c>
+      <c r="F61">
         <v>0.24</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>0.35</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>1.8148</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>0.94740000000000002</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>3.4729999999999999</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>0.89939999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62">
         <v>0.81</v>
@@ -2595,30 +2851,33 @@
         <v>0.53</v>
       </c>
       <c r="E62">
+        <v>0.98</v>
+      </c>
+      <c r="F62">
         <v>0.23</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>0.33</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>2.407</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>0.93030000000000002</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>3.6255999999999999</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63">
         <v>0.81</v>
@@ -2627,30 +2886,33 @@
         <v>0.43</v>
       </c>
       <c r="E63">
+        <v>0.93</v>
+      </c>
+      <c r="F63">
         <v>0.41</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>0.42</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>0.73560000000000003</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>0.97870000000000001</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>4.2363</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>0.87729999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>0.88</v>
@@ -2659,30 +2921,33 @@
         <v>0.54</v>
       </c>
       <c r="E64">
+        <v>0.99</v>
+      </c>
+      <c r="F64">
         <v>0.13</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>0.21</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>3.6774</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>0.89349999999999996</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>3.6638000000000002</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>0.89390000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>0.85</v>
@@ -2691,30 +2956,33 @@
         <v>0.45</v>
       </c>
       <c r="E65">
+        <v>0.97</v>
+      </c>
+      <c r="F65">
         <v>0.17</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>0.25</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>2.1255000000000002</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>0.93840000000000001</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>3.8927999999999998</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>0.88729999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>63</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" s="1">
         <v>0.84</v>
@@ -2723,30 +2991,33 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E66" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="F66" s="1">
         <v>0.71</v>
       </c>
-      <c r="F66" s="1">
+      <c r="G66" s="1">
         <v>0.42</v>
       </c>
-      <c r="G66" s="1">
+      <c r="H66" s="1">
         <v>8.5347000000000008</v>
       </c>
-      <c r="H66" s="1">
+      <c r="I66" s="1">
         <v>0.75290000000000001</v>
       </c>
-      <c r="I66" s="1">
+      <c r="J66" s="1">
         <v>7.4804000000000004</v>
       </c>
-      <c r="J66" s="1">
+      <c r="K66" s="1">
         <v>0.78339999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67">
         <v>0.62</v>
@@ -2754,31 +3025,34 @@
       <c r="D67">
         <v>0</v>
       </c>
-      <c r="E67">
-        <v>0</v>
+      <c r="E67" s="2">
+        <v>1</v>
       </c>
       <c r="F67">
         <v>0</v>
       </c>
       <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
         <v>4.0212000000000003</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>0.88360000000000005</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>3.7783000000000002</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>0.89059999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C68">
         <v>0.83</v>
@@ -2786,31 +3060,34 @@
       <c r="D68">
         <v>0.54</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="F68">
         <v>0.34</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>0.42</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>3.1903000000000001</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>0.90759999999999996</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>3.5493000000000001</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>0.8972</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C69">
         <v>0.69</v>
@@ -2818,31 +3095,34 @@
       <c r="D69">
         <v>0</v>
       </c>
-      <c r="E69">
-        <v>0</v>
+      <c r="E69" s="2">
+        <v>1</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
         <v>3.4885000000000002</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>0.89900000000000002</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>3.7401</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>0.89170000000000005</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C70">
         <v>0.77</v>
@@ -2850,63 +3130,69 @@
       <c r="D70">
         <v>0</v>
       </c>
-      <c r="E70">
-        <v>0</v>
+      <c r="E70" s="2">
+        <v>1</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
         <v>4.0403000000000002</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>0.88300000000000001</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>3.7401</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>0.89170000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>68</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" s="1">
+      <c r="B71" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="2">
         <v>0.76</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="2">
         <v>0.23</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="F71" s="2">
         <v>0.64</v>
       </c>
-      <c r="F71" s="1">
+      <c r="G71" s="2">
         <v>0.34</v>
       </c>
-      <c r="G71" s="1">
+      <c r="H71" s="2">
         <v>7.1284999999999998</v>
       </c>
-      <c r="H71" s="1">
+      <c r="I71" s="2">
         <v>0.79359999999999997</v>
       </c>
-      <c r="I71" s="1">
+      <c r="J71" s="2">
         <v>9.5412999999999997</v>
       </c>
-      <c r="J71" s="1">
+      <c r="K71" s="2">
         <v>0.72370000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C72">
         <v>0.84</v>
@@ -2914,31 +3200,34 @@
       <c r="D72">
         <v>0.3</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F72">
         <v>0.7</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>0.42</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>8.5130999999999997</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>0.75349999999999995</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>7.3658999999999999</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>0.78669999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C73">
         <v>0.69</v>
@@ -2946,31 +3235,34 @@
       <c r="D73">
         <v>0</v>
       </c>
-      <c r="E73">
-        <v>0</v>
+      <c r="E73" s="2">
+        <v>1</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
         <v>4.0308000000000002</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>0.88329999999999997</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>3.7783000000000002</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>0.89059999999999995</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C74">
         <v>0.7</v>
@@ -2978,31 +3270,34 @@
       <c r="D74">
         <v>0.67</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
+      <c r="F74">
         <v>0.04</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>0.08</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>3.9447999999999999</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>0.88580000000000003</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>3.6638000000000002</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>0.89390000000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C75">
         <v>0.76</v>
@@ -3010,31 +3305,34 @@
       <c r="D75">
         <v>0.4</v>
       </c>
-      <c r="E75">
-        <v>0.4</v>
+      <c r="E75" s="2">
+        <v>0.93</v>
       </c>
       <c r="F75">
         <v>0.4</v>
       </c>
       <c r="G75">
+        <v>0.4</v>
+      </c>
+      <c r="H75">
         <v>3.6993999999999998</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>0.89290000000000003</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>4.4653</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <v>0.87070000000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C76">
         <v>0.75</v>
@@ -3042,31 +3340,34 @@
       <c r="D76">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="F76">
         <v>0.39</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>0.32</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>5.6069000000000004</v>
       </c>
-      <c r="H76">
+      <c r="I76">
         <v>0.8377</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>6.0682</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <v>0.82430000000000003</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C77">
         <v>0.72</v>
@@ -3074,31 +3375,34 @@
       <c r="D77">
         <v>0.22</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="F77">
         <v>0.67</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>0.33</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>7.4530000000000003</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>0.78420000000000001</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>10.266400000000001</v>
       </c>
-      <c r="J77">
+      <c r="K77">
         <v>0.70279999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>75</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C78">
         <v>0.68</v>
@@ -3106,31 +3410,34 @@
       <c r="D78">
         <v>0.24</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F78">
         <v>0.27</v>
       </c>
-      <c r="F78">
+      <c r="G78">
         <v>0.25</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>3.3912</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <v>0.90180000000000005</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <v>5.9154999999999998</v>
       </c>
-      <c r="J78">
+      <c r="K78">
         <v>0.82869999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C79">
         <v>0.77</v>
@@ -3138,31 +3445,34 @@
       <c r="D79">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="F79">
         <v>0.42</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>0.35</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>5.3011999999999997</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>0.84650000000000003</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>5.9156000000000004</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>0.82869999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C80">
         <v>0.76</v>
@@ -3170,31 +3480,34 @@
       <c r="D80">
         <v>0.15</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F80">
         <v>0.89</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>0.26</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>18.225000000000001</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>0.4723</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>19.0063</v>
       </c>
-      <c r="J80">
+      <c r="K80">
         <v>0.44969999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C81">
         <v>0.7</v>
@@ -3202,31 +3515,34 @@
       <c r="D81">
         <v>0.4</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F81">
         <v>0.04</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>2.6987999999999999</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>0.92190000000000005</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>3.8163999999999998</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>0.88949999999999996</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82">
         <v>0.8</v>
@@ -3234,31 +3550,34 @@
       <c r="D82">
         <v>0.3</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="F82">
         <v>0.45</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>0.36</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>5.8170000000000002</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>0.83160000000000001</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>5.9919000000000002</v>
       </c>
-      <c r="J82">
+      <c r="K82">
         <v>0.82650000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>80</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C83">
         <v>0.79</v>
@@ -3266,31 +3585,34 @@
       <c r="D83">
         <v>0.18</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F83">
         <v>0.87</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>0.3</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>9.4542999999999999</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <v>0.72629999999999995</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>15.3424</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>0.55579999999999996</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C84">
         <v>0.76</v>
@@ -3298,31 +3620,34 @@
       <c r="D84">
         <v>0.2</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F84">
         <v>0.8</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>0.32</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>8.1074999999999999</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>0.76529999999999998</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>12.5182</v>
       </c>
-      <c r="J84">
+      <c r="K84">
         <v>0.63759999999999994</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C85">
         <v>0.81</v>
@@ -3330,31 +3655,34 @@
       <c r="D85">
         <v>0.31</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="F85">
         <v>0.45</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>0.37</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>5.5686999999999998</v>
       </c>
-      <c r="H85">
+      <c r="I85">
         <v>0.83879999999999999</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>5.8010999999999999</v>
       </c>
-      <c r="J85">
+      <c r="K85">
         <v>0.83199999999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C86">
         <v>0.73</v>
@@ -3362,31 +3690,34 @@
       <c r="D86">
         <v>0.11</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F86">
         <v>0.98</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>0.2</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>28.980399999999999</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>0.16089999999999999</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>29.578099999999999</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>0.14360000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C87">
         <v>0.71</v>
@@ -3394,27 +3725,882 @@
       <c r="D87">
         <v>0.11</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="F87">
         <v>0.91</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>0.2</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>15.847300000000001</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>0.54120000000000001</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>27.593499999999999</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>0.2011</v>
       </c>
     </row>
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88">
+        <v>0.92</v>
+      </c>
+      <c r="D88">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E88">
+        <v>0.97</v>
+      </c>
+      <c r="F88">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G88">
+        <v>0.38</v>
+      </c>
+      <c r="H88">
+        <v>2.4834000000000001</v>
+      </c>
+      <c r="I88">
+        <v>0.92810000000000004</v>
+      </c>
+      <c r="J88">
+        <v>3.5110999999999999</v>
+      </c>
+      <c r="K88">
+        <v>0.89829999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89" t="s">
+        <v>118</v>
+      </c>
+      <c r="C89">
+        <v>0.91</v>
+      </c>
+      <c r="D89">
+        <v>0.45</v>
+      </c>
+      <c r="E89">
+        <v>0.9</v>
+      </c>
+      <c r="F89">
+        <v>0.67</v>
+      </c>
+      <c r="G89">
+        <v>0.54</v>
+      </c>
+      <c r="H89">
+        <v>2.2446000000000002</v>
+      </c>
+      <c r="I89">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J89">
+        <v>4.3507999999999996</v>
+      </c>
+      <c r="K89">
+        <v>0.874</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90">
+        <v>0.91</v>
+      </c>
+      <c r="D90">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E90">
+        <v>0.95</v>
+      </c>
+      <c r="F90">
+        <v>0.48</v>
+      </c>
+      <c r="G90">
+        <v>0.51</v>
+      </c>
+      <c r="H90">
+        <v>1.6496</v>
+      </c>
+      <c r="I90">
+        <v>0.95220000000000005</v>
+      </c>
+      <c r="J90">
+        <v>3.4348000000000001</v>
+      </c>
+      <c r="K90">
+        <v>0.90049999999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91" t="s">
+        <v>97</v>
+      </c>
+      <c r="C91">
+        <v>0.92</v>
+      </c>
+      <c r="D91">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E91">
+        <v>0.97</v>
+      </c>
+      <c r="F91">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G91">
+        <v>0.38</v>
+      </c>
+      <c r="H91">
+        <v>2.4834000000000001</v>
+      </c>
+      <c r="I91">
+        <v>0.92810000000000004</v>
+      </c>
+      <c r="J91">
+        <v>3.5110999999999999</v>
+      </c>
+      <c r="K91">
+        <v>0.89829999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92" t="s">
+        <v>98</v>
+      </c>
+      <c r="C92">
+        <v>0.83</v>
+      </c>
+      <c r="D92">
+        <v>0.6</v>
+      </c>
+      <c r="E92">
+        <v>0.98</v>
+      </c>
+      <c r="F92">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G92">
+        <v>0.39</v>
+      </c>
+      <c r="H92">
+        <v>2.8559999999999999</v>
+      </c>
+      <c r="I92">
+        <v>0.9173</v>
+      </c>
+      <c r="J92">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="K92">
+        <v>0.90159999999999996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93" t="s">
+        <v>99</v>
+      </c>
+      <c r="C93">
+        <v>0.81</v>
+      </c>
+      <c r="D93">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E93">
+        <v>0.96</v>
+      </c>
+      <c r="F93">
+        <v>0.36</v>
+      </c>
+      <c r="G93">
+        <v>0.43</v>
+      </c>
+      <c r="H93">
+        <v>2.6177000000000001</v>
+      </c>
+      <c r="I93">
+        <v>0.92420000000000002</v>
+      </c>
+      <c r="J93">
+        <v>3.5110999999999999</v>
+      </c>
+      <c r="K93">
+        <v>0.89829999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94">
+        <v>0.91</v>
+      </c>
+      <c r="D94">
+        <v>0.54</v>
+      </c>
+      <c r="E94">
+        <v>0.97</v>
+      </c>
+      <c r="F94">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G94">
+        <v>0.36</v>
+      </c>
+      <c r="H94">
+        <v>2.5884999999999998</v>
+      </c>
+      <c r="I94">
+        <v>0.92510000000000003</v>
+      </c>
+      <c r="J94">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="K94">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95">
+        <v>0.89</v>
+      </c>
+      <c r="D95">
+        <v>0.42</v>
+      </c>
+      <c r="E95">
+        <v>0.89</v>
+      </c>
+      <c r="F95">
+        <v>0.65</v>
+      </c>
+      <c r="G95">
+        <v>0.51</v>
+      </c>
+      <c r="H95">
+        <v>2.5636999999999999</v>
+      </c>
+      <c r="I95">
+        <v>0.92579999999999996</v>
+      </c>
+      <c r="J95">
+        <v>4.7324999999999999</v>
+      </c>
+      <c r="K95">
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96" t="s">
+        <v>102</v>
+      </c>
+      <c r="C96">
+        <v>0.88</v>
+      </c>
+      <c r="D96">
+        <v>0.39</v>
+      </c>
+      <c r="E96">
+        <v>0.88</v>
+      </c>
+      <c r="F96">
+        <v>0.63</v>
+      </c>
+      <c r="G96">
+        <v>0.48</v>
+      </c>
+      <c r="H96">
+        <v>2.9205999999999999</v>
+      </c>
+      <c r="I96">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="J96">
+        <v>5.0759999999999996</v>
+      </c>
+      <c r="K96">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97" t="s">
+        <v>103</v>
+      </c>
+      <c r="C97">
+        <v>0.91</v>
+      </c>
+      <c r="D97">
+        <v>0.54</v>
+      </c>
+      <c r="E97">
+        <v>0.97</v>
+      </c>
+      <c r="F97">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G97">
+        <v>0.36</v>
+      </c>
+      <c r="H97">
+        <v>2.5884999999999998</v>
+      </c>
+      <c r="I97">
+        <v>0.92510000000000003</v>
+      </c>
+      <c r="J97">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="K97">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98">
+        <v>0.82</v>
+      </c>
+      <c r="D98">
+        <v>0.53</v>
+      </c>
+      <c r="E98">
+        <v>0.97</v>
+      </c>
+      <c r="F98">
+        <v>0.24</v>
+      </c>
+      <c r="G98">
+        <v>0.34</v>
+      </c>
+      <c r="H98">
+        <v>3.0087999999999999</v>
+      </c>
+      <c r="I98">
+        <v>0.91290000000000004</v>
+      </c>
+      <c r="J98">
+        <v>3.6255999999999999</v>
+      </c>
+      <c r="K98">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99" t="s">
+        <v>105</v>
+      </c>
+      <c r="C99">
+        <v>0.83</v>
+      </c>
+      <c r="D99">
+        <v>0.45</v>
+      </c>
+      <c r="E99">
+        <v>0.93</v>
+      </c>
+      <c r="F99">
+        <v>0.46</v>
+      </c>
+      <c r="G99">
+        <v>0.45</v>
+      </c>
+      <c r="H99">
+        <v>3.0503999999999998</v>
+      </c>
+      <c r="I99">
+        <v>0.91169999999999995</v>
+      </c>
+      <c r="J99">
+        <v>4.16</v>
+      </c>
+      <c r="K99">
+        <v>0.87960000000000005</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100">
+        <v>0.92</v>
+      </c>
+      <c r="D100">
+        <v>0.53</v>
+      </c>
+      <c r="E100">
+        <v>0.97</v>
+      </c>
+      <c r="F100">
+        <v>0.32</v>
+      </c>
+      <c r="G100">
+        <v>0.4</v>
+      </c>
+      <c r="H100">
+        <v>2.7031000000000001</v>
+      </c>
+      <c r="I100">
+        <v>0.92169999999999996</v>
+      </c>
+      <c r="J100">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="K100">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101" t="s">
+        <v>107</v>
+      </c>
+      <c r="C101">
+        <v>0.91</v>
+      </c>
+      <c r="D101">
+        <v>0.49</v>
+      </c>
+      <c r="E101">
+        <v>0.93</v>
+      </c>
+      <c r="F101">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G101">
+        <v>0.53</v>
+      </c>
+      <c r="H101">
+        <v>1.3035000000000001</v>
+      </c>
+      <c r="I101">
+        <v>0.96230000000000004</v>
+      </c>
+      <c r="J101">
+        <v>3.8165</v>
+      </c>
+      <c r="K101">
+        <v>0.88949999999999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102" t="s">
+        <v>108</v>
+      </c>
+      <c r="C102">
+        <v>0.91</v>
+      </c>
+      <c r="D102">
+        <v>0.54</v>
+      </c>
+      <c r="E102">
+        <v>0.96</v>
+      </c>
+      <c r="F102">
+        <v>0.44</v>
+      </c>
+      <c r="G102">
+        <v>0.49</v>
+      </c>
+      <c r="H102">
+        <v>1.6226</v>
+      </c>
+      <c r="I102">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="J102">
+        <v>3.4729999999999999</v>
+      </c>
+      <c r="K102">
+        <v>0.89939999999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103" t="s">
+        <v>109</v>
+      </c>
+      <c r="C103">
+        <v>0.92</v>
+      </c>
+      <c r="D103">
+        <v>0.53</v>
+      </c>
+      <c r="E103">
+        <v>0.97</v>
+      </c>
+      <c r="F103">
+        <v>0.32</v>
+      </c>
+      <c r="G103">
+        <v>0.4</v>
+      </c>
+      <c r="H103">
+        <v>2.7031000000000001</v>
+      </c>
+      <c r="I103">
+        <v>0.92169999999999996</v>
+      </c>
+      <c r="J103">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="K103">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>101</v>
+      </c>
+      <c r="B104" t="s">
+        <v>110</v>
+      </c>
+      <c r="C104">
+        <v>0.83</v>
+      </c>
+      <c r="D104">
+        <v>0.6</v>
+      </c>
+      <c r="E104">
+        <v>0.98</v>
+      </c>
+      <c r="F104">
+        <v>0.27</v>
+      </c>
+      <c r="G104">
+        <v>0.37</v>
+      </c>
+      <c r="H104">
+        <v>3.2570999999999999</v>
+      </c>
+      <c r="I104">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="J104">
+        <v>3.3965999999999998</v>
+      </c>
+      <c r="K104">
+        <v>0.90159999999999996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>102</v>
+      </c>
+      <c r="B105" t="s">
+        <v>111</v>
+      </c>
+      <c r="C105">
+        <v>0.82</v>
+      </c>
+      <c r="D105">
+        <v>0.53</v>
+      </c>
+      <c r="E105">
+        <v>0.97</v>
+      </c>
+      <c r="F105">
+        <v>0.3</v>
+      </c>
+      <c r="G105">
+        <v>0.38</v>
+      </c>
+      <c r="H105">
+        <v>2.1903999999999999</v>
+      </c>
+      <c r="I105">
+        <v>0.93659999999999999</v>
+      </c>
+      <c r="J105">
+        <v>3.6255999999999999</v>
+      </c>
+      <c r="K105">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>103</v>
+      </c>
+      <c r="B106" t="s">
+        <v>112</v>
+      </c>
+      <c r="C106">
+        <v>0.91</v>
+      </c>
+      <c r="D106">
+        <v>0.53</v>
+      </c>
+      <c r="E106">
+        <v>0.97</v>
+      </c>
+      <c r="F106">
+        <v>0.27</v>
+      </c>
+      <c r="G106">
+        <v>0.35</v>
+      </c>
+      <c r="H106">
+        <v>2.8751000000000002</v>
+      </c>
+      <c r="I106">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="J106">
+        <v>3.6255999999999999</v>
+      </c>
+      <c r="K106">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107" t="s">
+        <v>113</v>
+      </c>
+      <c r="C107">
+        <v>0.9</v>
+      </c>
+      <c r="D107">
+        <v>0.47</v>
+      </c>
+      <c r="E107">
+        <v>0.92</v>
+      </c>
+      <c r="F107">
+        <v>0.62</v>
+      </c>
+      <c r="G107">
+        <v>0.54</v>
+      </c>
+      <c r="H107">
+        <v>1.4982</v>
+      </c>
+      <c r="I107">
+        <v>0.95660000000000001</v>
+      </c>
+      <c r="J107">
+        <v>4.0072999999999999</v>
+      </c>
+      <c r="K107">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>105</v>
+      </c>
+      <c r="B108" t="s">
+        <v>114</v>
+      </c>
+      <c r="C108">
+        <v>0.89</v>
+      </c>
+      <c r="D108">
+        <v>0.43</v>
+      </c>
+      <c r="E108">
+        <v>0.9</v>
+      </c>
+      <c r="F108">
+        <v>0.63</v>
+      </c>
+      <c r="G108">
+        <v>0.51</v>
+      </c>
+      <c r="H108">
+        <v>1.6226</v>
+      </c>
+      <c r="I108">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="J108">
+        <v>4.5034999999999998</v>
+      </c>
+      <c r="K108">
+        <v>0.86960000000000004</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>106</v>
+      </c>
+      <c r="B109" t="s">
+        <v>115</v>
+      </c>
+      <c r="C109">
+        <v>0.91</v>
+      </c>
+      <c r="D109">
+        <v>0.53</v>
+      </c>
+      <c r="E109">
+        <v>0.97</v>
+      </c>
+      <c r="F109">
+        <v>0.27</v>
+      </c>
+      <c r="G109">
+        <v>0.35</v>
+      </c>
+      <c r="H109">
+        <v>2.8654999999999999</v>
+      </c>
+      <c r="I109">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="J109">
+        <v>3.6255999999999999</v>
+      </c>
+      <c r="K109">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>107</v>
+      </c>
+      <c r="B110" t="s">
+        <v>116</v>
+      </c>
+      <c r="C110">
+        <v>0.82</v>
+      </c>
+      <c r="D110">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E110">
+        <v>0.98</v>
+      </c>
+      <c r="F110">
+        <v>0.23</v>
+      </c>
+      <c r="G110">
+        <v>0.33</v>
+      </c>
+      <c r="H110">
+        <v>3.2284999999999999</v>
+      </c>
+      <c r="I110">
+        <v>0.90649999999999997</v>
+      </c>
+      <c r="J110">
+        <v>3.5874999999999999</v>
+      </c>
+      <c r="K110">
+        <v>0.89610000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>108</v>
+      </c>
+      <c r="B111" t="s">
+        <v>117</v>
+      </c>
+      <c r="C111">
+        <v>0.82</v>
+      </c>
+      <c r="D111">
+        <v>0.44</v>
+      </c>
+      <c r="E111">
+        <v>0.93</v>
+      </c>
+      <c r="F111">
+        <v>0.42</v>
+      </c>
+      <c r="G111">
+        <v>0.43</v>
+      </c>
+      <c r="H111">
+        <v>2.4283999999999999</v>
+      </c>
+      <c r="I111">
+        <v>0.92969999999999997</v>
+      </c>
+      <c r="J111">
+        <v>4.1981000000000002</v>
+      </c>
+      <c r="K111">
+        <v>0.87839999999999996</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J87">
+  <autoFilter ref="A3:K111" xr:uid="{BE32FFB3-C31A-4740-AC86-CD03484FED41}">
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="greaterThan" val="0.7"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="greaterThan" val="0.7"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K87">
     <sortCondition ref="A4:A87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test and Train Codes for Submission
</commit_message>
<xml_diff>
--- a/results/Model_Results_Summary.xlsx
+++ b/results/Model_Results_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AIML\Capstone Project Loan Processing\CodeBase\loan-processing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAD7A0C-68B6-495F-A141-6E74341DAF40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A95679-862A-4C3D-9902-6E2F8E9D7E4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00CAFC6D-E7ED-4D37-8A6B-16C8E85EC937}"/>
   </bookViews>
@@ -758,8 +758,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A3:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H116" sqref="H116"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4588,7 +4588,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:K111" xr:uid="{BE32FFB3-C31A-4740-AC86-CD03484FED41}">
+  <autoFilter ref="A3:K111" xr:uid="{24ADA6ED-7A6D-4481-998B-06BAD472C3F0}">
     <filterColumn colId="4">
       <customFilters>
         <customFilter operator="greaterThan" val="0.7"/>

</xml_diff>